<commit_message>
#4 pk dashboard final 3
</commit_message>
<xml_diff>
--- a/public/datafiles/ward_coordinates.xlsx
+++ b/public/datafiles/ward_coordinates.xlsx
@@ -1,16 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhavani\Desktop\shudh.ANVI\public\datafiles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2280440B-8582-474E-A238-7B8690B5570C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet name="vertices" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="vertices" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="13">
   <si>
     <t>id</t>
   </si>
@@ -54,29 +64,24 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="DD/MM/YY" numFmtId="165"/>
-    <numFmt formatCode="DD/MM/YYYY\ HH:MM:SS" numFmtId="166"/>
-    <numFmt formatCode="HH:MM:SS" numFmtId="167"/>
-    <numFmt formatCode="DD/MM/YYYY\ HH:MM:SS.000" numFmtId="168"/>
-    <numFmt formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;" numFmtId="169"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <sz val="10"/>
     </font>
   </fonts>
-  <fills count="1">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -85,41 +90,336 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="164">
-</xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="164" xfId="0"/>
-    <xf numFmtId="165" xfId="0"/>
-    <xf numFmtId="166" xfId="0"/>
-    <xf numFmtId="167" xfId="0"/>
-    <xf numFmtId="168" xfId="0"/>
-    <xf numFmtId="169" xfId="0"/>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L73"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1024" width="15"/>
-    <col min="2" max="1024" width="15"/>
-    <col min="3" max="1024" width="15"/>
-    <col min="4" max="1024" width="15"/>
-    <col min="5" max="1024" width="15"/>
-    <col min="6" max="1024" width="15"/>
-    <col min="7" max="1024" width="15"/>
-    <col min="8" max="1024" width="15"/>
-    <col min="9" max="1024" width="15"/>
-    <col min="10" max="1024" width="15"/>
-    <col min="11" max="1024" width="15"/>
-    <col min="12" max="1024" width="15"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -157,7 +457,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -168,7 +468,7 @@
         <v>726916.255</v>
       </c>
       <c r="D2">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -186,16 +486,16 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>266.9553634181287</v>
+        <v>266.95536341812868</v>
       </c>
       <c r="K2">
-        <v>78.49270799999999</v>
+        <v>78.492707999999993</v>
       </c>
       <c r="L2">
         <v>17.47231</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -206,7 +506,7 @@
         <v>726916.255</v>
       </c>
       <c r="D3">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -221,19 +521,19 @@
         <v>1</v>
       </c>
       <c r="I3">
-        <v>0.00054155186943</v>
+        <v>5.4155186943000003E-4</v>
       </c>
       <c r="J3">
-        <v>267.8225950666912</v>
+        <v>267.82259506669118</v>
       </c>
       <c r="K3">
-        <v>78.492169</v>
+        <v>78.492169000000004</v>
       </c>
       <c r="L3">
-        <v>17.47225</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>17.472249999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -244,7 +544,7 @@
         <v>726916.255</v>
       </c>
       <c r="D4">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -259,19 +559,19 @@
         <v>2</v>
       </c>
       <c r="I4">
-        <v>0.00160429916971</v>
+        <v>1.60429916971E-3</v>
       </c>
       <c r="J4">
-        <v>285.7588582177599</v>
+        <v>285.75885821775989</v>
       </c>
       <c r="K4">
         <v>78.491107</v>
       </c>
       <c r="L4">
-        <v>17.47228</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>17.472280000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -282,7 +582,7 @@
         <v>726916.255</v>
       </c>
       <c r="D5">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -297,19 +597,19 @@
         <v>3</v>
       </c>
       <c r="I5">
-        <v>0.0017014363317</v>
+        <v>1.7014363316999999E-3</v>
       </c>
       <c r="J5">
-        <v>259.6982173566329</v>
+        <v>259.69821735663288</v>
       </c>
       <c r="K5">
-        <v>78.491023</v>
+        <v>78.491022999999998</v>
       </c>
       <c r="L5">
-        <v>17.47233</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>17.472329999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -320,7 +620,7 @@
         <v>726916.255</v>
       </c>
       <c r="D6">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -335,19 +635,19 @@
         <v>4</v>
       </c>
       <c r="I6">
-        <v>0.00209810924321</v>
+        <v>2.0981092432099998E-3</v>
       </c>
       <c r="J6">
-        <v>243.5928205517476</v>
+        <v>243.59282055174759</v>
       </c>
       <c r="K6">
-        <v>78.49077</v>
+        <v>78.490769999999998</v>
       </c>
       <c r="L6">
         <v>17.47203</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -358,7 +658,7 @@
         <v>726916.255</v>
       </c>
       <c r="D7">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E7">
         <v>5</v>
@@ -373,19 +673,19 @@
         <v>5</v>
       </c>
       <c r="I7">
-        <v>0.00285754819332</v>
+        <v>2.8575481933199999E-3</v>
       </c>
       <c r="J7">
-        <v>270.1687595690867</v>
+        <v>270.16875956908672</v>
       </c>
       <c r="K7">
-        <v>78.490011</v>
+        <v>78.490010999999996</v>
       </c>
       <c r="L7">
-        <v>17.47199</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>17.471990000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -396,7 +696,7 @@
         <v>726916.255</v>
       </c>
       <c r="D8">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E8">
         <v>6</v>
@@ -411,19 +711,19 @@
         <v>6</v>
       </c>
       <c r="I8">
-        <v>0.0041911416434</v>
+        <v>4.1911416433999997E-3</v>
       </c>
       <c r="J8">
-        <v>267.1000566143734</v>
+        <v>267.10005661437339</v>
       </c>
       <c r="K8">
-        <v>78.488679</v>
+        <v>78.488679000000005</v>
       </c>
       <c r="L8">
-        <v>17.47206</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>17.472059999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -434,7 +734,7 @@
         <v>726916.255</v>
       </c>
       <c r="D9">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E9">
         <v>7</v>
@@ -449,19 +749,19 @@
         <v>7</v>
       </c>
       <c r="I9">
-        <v>0.00451511898538</v>
+        <v>4.5151189853800001E-3</v>
       </c>
       <c r="J9">
-        <v>222.716509802446</v>
+        <v>222.71650980244601</v>
       </c>
       <c r="K9">
-        <v>78.488359</v>
+        <v>78.488359000000003</v>
       </c>
       <c r="L9">
-        <v>17.47201</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>17.472010000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -472,7 +772,7 @@
         <v>726916.255</v>
       </c>
       <c r="D10">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E10">
         <v>8</v>
@@ -487,19 +787,19 @@
         <v>8</v>
       </c>
       <c r="I10">
-        <v>0.00475695805111</v>
+        <v>4.7569580511100003E-3</v>
       </c>
       <c r="J10">
         <v>226.9989829928472</v>
       </c>
       <c r="K10">
-        <v>78.488342</v>
+        <v>78.488342000000003</v>
       </c>
       <c r="L10">
-        <v>17.47177</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>17.471769999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -510,7 +810,7 @@
         <v>726916.255</v>
       </c>
       <c r="D11">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E11">
         <v>9</v>
@@ -525,19 +825,19 @@
         <v>9</v>
       </c>
       <c r="I11">
-        <v>0.00516162867466</v>
+        <v>5.1616286746600003E-3</v>
       </c>
       <c r="J11">
-        <v>266.6002707846546</v>
+        <v>266.60027078465458</v>
       </c>
       <c r="K11">
-        <v>78.487937</v>
+        <v>78.487937000000002</v>
       </c>
       <c r="L11">
-        <v>17.47177</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>17.471769999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -548,7 +848,7 @@
         <v>726916.255</v>
       </c>
       <c r="D12">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E12">
         <v>10</v>
@@ -563,19 +863,19 @@
         <v>10</v>
       </c>
       <c r="I12">
-        <v>0.00692762226786</v>
+        <v>6.9276222678600003E-3</v>
       </c>
       <c r="J12">
-        <v>231.0233641592152</v>
+        <v>231.02336415921519</v>
       </c>
       <c r="K12">
-        <v>78.48618399999999</v>
+        <v>78.486183999999994</v>
       </c>
       <c r="L12">
         <v>17.47156</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -586,7 +886,7 @@
         <v>726916.255</v>
       </c>
       <c r="D13">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E13">
         <v>11</v>
@@ -601,19 +901,19 @@
         <v>11</v>
       </c>
       <c r="I13">
-        <v>0.00765838664769</v>
+        <v>7.6583866476900003E-3</v>
       </c>
       <c r="J13">
-        <v>198.224328460606</v>
+        <v>198.22432846060599</v>
       </c>
       <c r="K13">
-        <v>78.48594799999999</v>
+        <v>78.485947999999993</v>
       </c>
       <c r="L13">
-        <v>17.47087</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>17.470870000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -624,7 +924,7 @@
         <v>726916.255</v>
       </c>
       <c r="D14">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E14">
         <v>12</v>
@@ -639,19 +939,19 @@
         <v>12</v>
       </c>
       <c r="I14">
-        <v>0.00894077838191</v>
+        <v>8.9407783819100001E-3</v>
       </c>
       <c r="J14">
-        <v>240.0083598758551</v>
+        <v>240.00835987585509</v>
       </c>
       <c r="K14">
-        <v>78.48556000000001</v>
+        <v>78.485560000000007</v>
       </c>
       <c r="L14">
-        <v>17.46964</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>17.469639999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -662,7 +962,7 @@
         <v>726916.255</v>
       </c>
       <c r="D15">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E15">
         <v>13</v>
@@ -677,19 +977,19 @@
         <v>13</v>
       </c>
       <c r="I15">
-        <v>0.01096077759025</v>
+        <v>1.096077759025E-2</v>
       </c>
       <c r="J15">
-        <v>329.5444220017497</v>
+        <v>329.54442200174969</v>
       </c>
       <c r="K15">
         <v>78.483587</v>
       </c>
       <c r="L15">
-        <v>17.47008</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>17.470079999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -700,7 +1000,7 @@
         <v>726916.255</v>
       </c>
       <c r="D16">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E16">
         <v>14</v>
@@ -715,19 +1015,19 @@
         <v>14</v>
       </c>
       <c r="I16">
-        <v>0.01178346293661</v>
+        <v>1.1783462936609999E-2</v>
       </c>
       <c r="J16">
-        <v>20.58927599822974</v>
+        <v>20.589275998229741</v>
       </c>
       <c r="K16">
-        <v>78.483823</v>
+        <v>78.483823000000001</v>
       </c>
       <c r="L16">
-        <v>17.47087</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>17.470870000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
@@ -738,7 +1038,7 @@
         <v>726916.255</v>
       </c>
       <c r="D17">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E17">
         <v>15</v>
@@ -753,19 +1053,19 @@
         <v>15</v>
       </c>
       <c r="I17">
-        <v>0.01218999767299</v>
+        <v>1.218999767299E-2</v>
       </c>
       <c r="J17">
         <v>31.99137749102567</v>
       </c>
       <c r="K17">
-        <v>78.483992</v>
+        <v>78.483992000000001</v>
       </c>
       <c r="L17">
-        <v>17.47124</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>17.471240000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -776,7 +1076,7 @@
         <v>726916.255</v>
       </c>
       <c r="D18">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E18">
         <v>16</v>
@@ -791,19 +1091,19 @@
         <v>16</v>
       </c>
       <c r="I18">
-        <v>0.01277343958824</v>
+        <v>1.2773439588239999E-2</v>
       </c>
       <c r="J18">
-        <v>23.32458455371773</v>
+        <v>23.324584553717731</v>
       </c>
       <c r="K18">
-        <v>78.484363</v>
+        <v>78.484363000000002</v>
       </c>
       <c r="L18">
-        <v>17.47169</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>17.471689999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
@@ -814,7 +1114,7 @@
         <v>726916.255</v>
       </c>
       <c r="D19">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E19">
         <v>17</v>
@@ -829,19 +1129,19 @@
         <v>17</v>
       </c>
       <c r="I19">
-        <v>0.01317869318371</v>
+        <v>1.317869318371E-2</v>
       </c>
       <c r="J19">
         <v>13.84861168653898</v>
       </c>
       <c r="K19">
-        <v>78.484413</v>
+        <v>78.484413000000004</v>
       </c>
       <c r="L19">
-        <v>17.47209</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>17.472090000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
@@ -852,7 +1152,7 @@
         <v>726916.255</v>
       </c>
       <c r="D20">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E20">
         <v>18</v>
@@ -867,19 +1167,19 @@
         <v>18</v>
       </c>
       <c r="I20">
-        <v>0.01495482649586</v>
+        <v>1.495482649586E-2</v>
       </c>
       <c r="J20">
-        <v>20.35782852883821</v>
+        <v>20.357828528838208</v>
       </c>
       <c r="K20">
-        <v>78.48503599999999</v>
+        <v>78.485035999999994</v>
       </c>
       <c r="L20">
-        <v>17.47375</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>17.473749999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
@@ -890,7 +1190,7 @@
         <v>726916.255</v>
       </c>
       <c r="D21">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E21">
         <v>19</v>
@@ -905,19 +1205,19 @@
         <v>19</v>
       </c>
       <c r="I21">
-        <v>0.01811334731571</v>
+        <v>1.8113347315710002E-2</v>
       </c>
       <c r="J21">
-        <v>19.50215632283968</v>
+        <v>19.502156322839681</v>
       </c>
       <c r="K21">
-        <v>78.486126</v>
+        <v>78.486125999999999</v>
       </c>
       <c r="L21">
         <v>17.47672</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -928,7 +1228,7 @@
         <v>726916.255</v>
       </c>
       <c r="D22">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E22">
         <v>20</v>
@@ -943,19 +1243,19 @@
         <v>20</v>
       </c>
       <c r="I22">
-        <v>0.01978003562771</v>
+        <v>1.978003562771E-2</v>
       </c>
       <c r="J22">
-        <v>66.49449741970972</v>
+        <v>66.494497419709717</v>
       </c>
       <c r="K22">
-        <v>78.486664</v>
+        <v>78.486664000000005</v>
       </c>
       <c r="L22">
-        <v>17.4783</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>17.478300000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -966,7 +1266,7 @@
         <v>726916.255</v>
       </c>
       <c r="D23">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E23">
         <v>21</v>
@@ -981,10 +1281,10 @@
         <v>21</v>
       </c>
       <c r="I23">
-        <v>0.02016528937794</v>
+        <v>2.0165289377940002E-2</v>
       </c>
       <c r="J23">
-        <v>82.59493961081689</v>
+        <v>82.594939610816894</v>
       </c>
       <c r="K23">
         <v>78.487015</v>
@@ -993,7 +1293,7 @@
         <v>17.47814</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1004,7 +1304,7 @@
         <v>726916.255</v>
       </c>
       <c r="D24">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E24">
         <v>22</v>
@@ -1019,19 +1319,19 @@
         <v>22</v>
       </c>
       <c r="I24">
-        <v>0.02104299930228</v>
+        <v>2.1042999302279999E-2</v>
       </c>
       <c r="J24">
-        <v>78.61445256827687</v>
+        <v>78.614452568276874</v>
       </c>
       <c r="K24">
-        <v>78.487697</v>
+        <v>78.487696999999997</v>
       </c>
       <c r="L24">
         <v>17.47869</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1</v>
       </c>
@@ -1042,7 +1342,7 @@
         <v>726916.255</v>
       </c>
       <c r="D25">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E25">
         <v>23</v>
@@ -1057,19 +1357,19 @@
         <v>23</v>
       </c>
       <c r="I25">
-        <v>0.02344902521505</v>
+        <v>2.344902521505E-2</v>
       </c>
       <c r="J25">
-        <v>131.4314777025835</v>
+        <v>131.43147770258349</v>
       </c>
       <c r="K25">
-        <v>78.490008</v>
+        <v>78.490008000000003</v>
       </c>
       <c r="L25">
-        <v>17.47802</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>17.478020000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1080,7 +1380,7 @@
         <v>726916.255</v>
       </c>
       <c r="D26">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E26">
         <v>24</v>
@@ -1095,19 +1395,19 @@
         <v>24</v>
       </c>
       <c r="I26">
-        <v>0.02463951838668</v>
+        <v>2.463951838668E-2</v>
       </c>
       <c r="J26">
-        <v>157.7656752526204</v>
+        <v>157.76567525262041</v>
       </c>
       <c r="K26">
-        <v>78.49048000000001</v>
+        <v>78.490480000000005</v>
       </c>
       <c r="L26">
         <v>17.47692</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
@@ -1118,7 +1418,7 @@
         <v>726916.255</v>
       </c>
       <c r="D27">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E27">
         <v>25</v>
@@ -1133,19 +1433,19 @@
         <v>25</v>
       </c>
       <c r="I27">
-        <v>0.025076034031</v>
+        <v>2.5076034031000002E-2</v>
       </c>
       <c r="J27">
         <v>142.7258753972408</v>
       </c>
       <c r="K27">
-        <v>78.49063700000001</v>
+        <v>78.490637000000007</v>
       </c>
       <c r="L27">
-        <v>17.47652</v>
-      </c>
-    </row>
-    <row r="28">
+        <v>17.476520000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1156,7 +1456,7 @@
         <v>726916.255</v>
       </c>
       <c r="D28">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E28">
         <v>26</v>
@@ -1171,19 +1471,19 @@
         <v>26</v>
       </c>
       <c r="I28">
-        <v>0.0255796122062</v>
+        <v>2.55796122062E-2</v>
       </c>
       <c r="J28">
-        <v>106.4661672610876</v>
+        <v>106.46616726108761</v>
       </c>
       <c r="K28">
-        <v>78.491041</v>
+        <v>78.491040999999996</v>
       </c>
       <c r="L28">
-        <v>17.47622</v>
-      </c>
-    </row>
-    <row r="29">
+        <v>17.476220000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1194,7 +1494,7 @@
         <v>726916.255</v>
       </c>
       <c r="D29">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E29">
         <v>27</v>
@@ -1209,19 +1509,19 @@
         <v>27</v>
       </c>
       <c r="I29">
-        <v>0.02591732134388</v>
+        <v>2.5917321343880001E-2</v>
       </c>
       <c r="J29">
-        <v>57.01242594316114</v>
+        <v>57.012425943161141</v>
       </c>
       <c r="K29">
-        <v>78.491378</v>
+        <v>78.491377999999997</v>
       </c>
       <c r="L29">
-        <v>17.47624</v>
-      </c>
-    </row>
-    <row r="30">
+        <v>17.476240000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1232,7 +1532,7 @@
         <v>726916.255</v>
       </c>
       <c r="D30">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E30">
         <v>28</v>
@@ -1247,19 +1547,19 @@
         <v>28</v>
       </c>
       <c r="I30">
-        <v>0.0260587987153</v>
+        <v>2.6058798715300001E-2</v>
       </c>
       <c r="J30">
         <v>18.95469051757296</v>
       </c>
       <c r="K30">
-        <v>78.491444</v>
+        <v>78.491444000000001</v>
       </c>
       <c r="L30">
         <v>17.47636</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1</v>
       </c>
@@ -1270,7 +1570,7 @@
         <v>726916.255</v>
       </c>
       <c r="D31">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E31">
         <v>29</v>
@@ -1285,19 +1585,19 @@
         <v>29</v>
       </c>
       <c r="I31">
-        <v>0.02679734469054</v>
+        <v>2.6797344690540001E-2</v>
       </c>
       <c r="J31">
         <v>19.60419381719846</v>
       </c>
       <c r="K31">
-        <v>78.491575</v>
+        <v>78.491574999999997</v>
       </c>
       <c r="L31">
         <v>17.47709</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
@@ -1308,7 +1608,7 @@
         <v>726916.255</v>
       </c>
       <c r="D32">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E32">
         <v>30</v>
@@ -1323,19 +1623,19 @@
         <v>30</v>
       </c>
       <c r="I32">
-        <v>0.02705398927575</v>
+        <v>2.705398927575E-2</v>
       </c>
       <c r="J32">
-        <v>68.04485307011136</v>
+        <v>68.044853070111358</v>
       </c>
       <c r="K32">
-        <v>78.49169999999999</v>
+        <v>78.491699999999994</v>
       </c>
       <c r="L32">
-        <v>17.47732</v>
-      </c>
-    </row>
-    <row r="33">
+        <v>17.477319999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1</v>
       </c>
@@ -1346,7 +1646,7 @@
         <v>726916.255</v>
       </c>
       <c r="D33">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E33">
         <v>31</v>
@@ -1361,19 +1661,19 @@
         <v>31</v>
       </c>
       <c r="I33">
-        <v>0.02786444200093</v>
+        <v>2.7864442000929999E-2</v>
       </c>
       <c r="J33">
-        <v>143.5636699868194</v>
+        <v>143.56366998681941</v>
       </c>
       <c r="K33">
-        <v>78.492474</v>
+        <v>78.492474000000001</v>
       </c>
       <c r="L33">
-        <v>17.47708</v>
-      </c>
-    </row>
-    <row r="34">
+        <v>17.477080000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1</v>
       </c>
@@ -1384,7 +1684,7 @@
         <v>726916.255</v>
       </c>
       <c r="D34">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E34">
         <v>32</v>
@@ -1399,19 +1699,19 @@
         <v>32</v>
       </c>
       <c r="I34">
-        <v>0.02806902115201</v>
+        <v>2.8069021152010001E-2</v>
       </c>
       <c r="J34">
-        <v>170.0621467159947</v>
+        <v>170.06214671599469</v>
       </c>
       <c r="K34">
-        <v>78.492474</v>
+        <v>78.492474000000001</v>
       </c>
       <c r="L34">
-        <v>17.47687</v>
-      </c>
-    </row>
-    <row r="35">
+        <v>17.476870000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1</v>
       </c>
@@ -1422,7 +1722,7 @@
         <v>726916.255</v>
       </c>
       <c r="D35">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E35">
         <v>33</v>
@@ -1437,19 +1737,19 @@
         <v>33</v>
       </c>
       <c r="I35">
-        <v>0.02841949848558</v>
+        <v>2.8419498485580001E-2</v>
       </c>
       <c r="J35">
         <v>183.8938310684926</v>
       </c>
       <c r="K35">
-        <v>78.492593</v>
+        <v>78.492592999999999</v>
       </c>
       <c r="L35">
         <v>17.47654</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1</v>
       </c>
@@ -1460,7 +1760,7 @@
         <v>726916.255</v>
       </c>
       <c r="D36">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E36">
         <v>34</v>
@@ -1475,19 +1775,19 @@
         <v>34</v>
       </c>
       <c r="I36">
-        <v>0.02880447080755</v>
+        <v>2.8804470807550001E-2</v>
       </c>
       <c r="J36">
         <v>163.7230500921826</v>
       </c>
       <c r="K36">
-        <v>78.49241499999999</v>
+        <v>78.492414999999994</v>
       </c>
       <c r="L36">
-        <v>17.4762</v>
-      </c>
-    </row>
-    <row r="37">
+        <v>17.476199999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1</v>
       </c>
@@ -1498,7 +1798,7 @@
         <v>726916.255</v>
       </c>
       <c r="D37">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E37">
         <v>35</v>
@@ -1513,19 +1813,19 @@
         <v>35</v>
       </c>
       <c r="I37">
-        <v>0.02901040494292</v>
+        <v>2.9010404942919999E-2</v>
       </c>
       <c r="J37">
-        <v>85.65132728284266</v>
+        <v>85.651327282842658</v>
       </c>
       <c r="K37">
-        <v>78.492593</v>
+        <v>78.492592999999999</v>
       </c>
       <c r="L37">
-        <v>17.4761</v>
-      </c>
-    </row>
-    <row r="38">
+        <v>17.476099999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1</v>
       </c>
@@ -1536,7 +1836,7 @@
         <v>726916.255</v>
       </c>
       <c r="D38">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E38">
         <v>36</v>
@@ -1551,19 +1851,19 @@
         <v>36</v>
       </c>
       <c r="I38">
-        <v>0.02919305977748</v>
+        <v>2.9193059777480001E-2</v>
       </c>
       <c r="J38">
-        <v>67.49510409984723</v>
+        <v>67.495104099847225</v>
       </c>
       <c r="K38">
-        <v>78.49273599999999</v>
+        <v>78.492735999999994</v>
       </c>
       <c r="L38">
-        <v>17.47621</v>
-      </c>
-    </row>
-    <row r="39">
+        <v>17.476209999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1</v>
       </c>
@@ -1574,7 +1874,7 @@
         <v>726916.255</v>
       </c>
       <c r="D39">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E39">
         <v>37</v>
@@ -1589,19 +1889,19 @@
         <v>37</v>
       </c>
       <c r="I39">
-        <v>0.02949289373991</v>
+        <v>2.9492893739910001E-2</v>
       </c>
       <c r="J39">
-        <v>63.36257189209774</v>
+        <v>63.362571892097741</v>
       </c>
       <c r="K39">
-        <v>78.49303399999999</v>
+        <v>78.493033999999994</v>
       </c>
       <c r="L39">
         <v>17.47625</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1</v>
       </c>
@@ -1612,7 +1912,7 @@
         <v>726916.255</v>
       </c>
       <c r="D40">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E40">
         <v>38</v>
@@ -1627,19 +1927,19 @@
         <v>38</v>
       </c>
       <c r="I40">
-        <v>0.03010150039956</v>
+        <v>3.0101500399559999E-2</v>
       </c>
       <c r="J40">
-        <v>76.70049554656276</v>
+        <v>76.700495546562763</v>
       </c>
       <c r="K40">
-        <v>78.49345099999999</v>
+        <v>78.493450999999993</v>
       </c>
       <c r="L40">
-        <v>17.47669</v>
-      </c>
-    </row>
-    <row r="41">
+        <v>17.476690000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1</v>
       </c>
@@ -1650,7 +1950,7 @@
         <v>726916.255</v>
       </c>
       <c r="D41">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E41">
         <v>39</v>
@@ -1665,10 +1965,10 @@
         <v>39</v>
       </c>
       <c r="I41">
-        <v>0.03026649763535</v>
+        <v>3.0266497635350002E-2</v>
       </c>
       <c r="J41">
-        <v>74.16199086317958</v>
+        <v>74.161990863179582</v>
       </c>
       <c r="K41">
         <v>78.493606</v>
@@ -1677,7 +1977,7 @@
         <v>17.47663</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1</v>
       </c>
@@ -1688,7 +1988,7 @@
         <v>726916.255</v>
       </c>
       <c r="D42">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E42">
         <v>40</v>
@@ -1703,19 +2003,19 @@
         <v>40</v>
       </c>
       <c r="I42">
-        <v>0.03072915948197</v>
+        <v>3.0729159481970001E-2</v>
       </c>
       <c r="J42">
-        <v>80.95417471860124</v>
+        <v>80.954174718601237</v>
       </c>
       <c r="K42">
-        <v>78.493892</v>
+        <v>78.493892000000002</v>
       </c>
       <c r="L42">
         <v>17.477</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1</v>
       </c>
@@ -1726,7 +2026,7 @@
         <v>726916.255</v>
       </c>
       <c r="D43">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E43">
         <v>41</v>
@@ -1741,7 +2041,7 @@
         <v>41</v>
       </c>
       <c r="I43">
-        <v>0.03087243410308</v>
+        <v>3.087243410308E-2</v>
       </c>
       <c r="J43">
         <v>110.9770011496983</v>
@@ -1753,7 +2053,7 @@
         <v>17.47692</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1</v>
       </c>
@@ -1764,7 +2064,7 @@
         <v>726916.255</v>
       </c>
       <c r="D44">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E44">
         <v>42</v>
@@ -1779,19 +2079,19 @@
         <v>42</v>
       </c>
       <c r="I44">
-        <v>0.03126973267401</v>
+        <v>3.1269732674010002E-2</v>
       </c>
       <c r="J44">
-        <v>70.19112102158417</v>
+        <v>70.191121021584166</v>
       </c>
       <c r="K44">
-        <v>78.494404</v>
+        <v>78.494404000000003</v>
       </c>
       <c r="L44">
-        <v>17.47686</v>
-      </c>
-    </row>
-    <row r="45">
+        <v>17.476859999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1</v>
       </c>
@@ -1802,7 +2102,7 @@
         <v>726916.255</v>
       </c>
       <c r="D45">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E45">
         <v>43</v>
@@ -1817,19 +2117,19 @@
         <v>43</v>
       </c>
       <c r="I45">
-        <v>0.03160703899249</v>
+        <v>3.1607038992489997E-2</v>
       </c>
       <c r="J45">
-        <v>26.33305844814693</v>
+        <v>26.333058448146929</v>
       </c>
       <c r="K45">
-        <v>78.494631</v>
+        <v>78.494630999999998</v>
       </c>
       <c r="L45">
         <v>17.47711</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1</v>
       </c>
@@ -1840,7 +2140,7 @@
         <v>726916.255</v>
       </c>
       <c r="D46">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E46">
         <v>44</v>
@@ -1855,19 +2155,19 @@
         <v>44</v>
       </c>
       <c r="I46">
-        <v>0.03212612056084</v>
+        <v>3.2126120560840001E-2</v>
       </c>
       <c r="J46">
-        <v>8.945252622333051</v>
+        <v>8.9452526223330509</v>
       </c>
       <c r="K46">
         <v>78.494726</v>
       </c>
       <c r="L46">
-        <v>17.47762</v>
-      </c>
-    </row>
-    <row r="47">
+        <v>17.477620000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1</v>
       </c>
@@ -1878,7 +2178,7 @@
         <v>726916.255</v>
       </c>
       <c r="D47">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E47">
         <v>45</v>
@@ -1893,19 +2193,19 @@
         <v>45</v>
       </c>
       <c r="I47">
-        <v>0.03314610101258</v>
+        <v>3.3146101012579997E-2</v>
       </c>
       <c r="J47">
-        <v>359.0602780414183</v>
+        <v>359.06027804141831</v>
       </c>
       <c r="K47">
-        <v>78.494857</v>
+        <v>78.494856999999996</v>
       </c>
       <c r="L47">
-        <v>17.47863</v>
-      </c>
-    </row>
-    <row r="48">
+        <v>17.478629999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1</v>
       </c>
@@ -1916,7 +2216,7 @@
         <v>726916.255</v>
       </c>
       <c r="D48">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E48">
         <v>46</v>
@@ -1931,19 +2231,19 @@
         <v>46</v>
       </c>
       <c r="I48">
-        <v>0.03366430027352</v>
+        <v>3.3664300273519999E-2</v>
       </c>
       <c r="J48">
-        <v>356.6193665862301</v>
+        <v>356.61936658623011</v>
       </c>
       <c r="K48">
-        <v>78.494773</v>
+        <v>78.494772999999995</v>
       </c>
       <c r="L48">
-        <v>17.47914</v>
-      </c>
-    </row>
-    <row r="49">
+        <v>17.479140000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>1</v>
       </c>
@@ -1954,7 +2254,7 @@
         <v>726916.255</v>
       </c>
       <c r="D49">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E49">
         <v>47</v>
@@ -1969,19 +2269,19 @@
         <v>47</v>
       </c>
       <c r="I49">
-        <v>0.03421035762185</v>
+        <v>3.4210357621849999E-2</v>
       </c>
       <c r="J49">
         <v>45.9329327871543</v>
       </c>
       <c r="K49">
-        <v>78.49479700000001</v>
+        <v>78.494797000000005</v>
       </c>
       <c r="L49">
-        <v>17.47969</v>
-      </c>
-    </row>
-    <row r="50">
+        <v>17.479690000000002</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>1</v>
       </c>
@@ -1992,7 +2292,7 @@
         <v>726916.255</v>
       </c>
       <c r="D50">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E50">
         <v>48</v>
@@ -2007,19 +2307,19 @@
         <v>48</v>
       </c>
       <c r="I50">
-        <v>0.0352351586109</v>
+        <v>3.52351586109E-2</v>
       </c>
       <c r="J50">
-        <v>135.7024988268711</v>
+        <v>135.70249882687111</v>
       </c>
       <c r="K50">
-        <v>78.495822</v>
+        <v>78.495822000000004</v>
       </c>
       <c r="L50">
-        <v>17.4797</v>
-      </c>
-    </row>
-    <row r="51">
+        <v>17.479700000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>1</v>
       </c>
@@ -2030,7 +2330,7 @@
         <v>726916.255</v>
       </c>
       <c r="D51">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E51">
         <v>49</v>
@@ -2045,19 +2345,19 @@
         <v>49</v>
       </c>
       <c r="I51">
-        <v>0.03651260288701</v>
+        <v>3.6512602887009998E-2</v>
       </c>
       <c r="J51">
-        <v>143.7475514061051</v>
+        <v>143.74755140610509</v>
       </c>
       <c r="K51">
-        <v>78.49577600000001</v>
+        <v>78.495776000000006</v>
       </c>
       <c r="L51">
         <v>17.47842</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1</v>
       </c>
@@ -2068,7 +2368,7 @@
         <v>726916.255</v>
       </c>
       <c r="D52">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E52">
         <v>50</v>
@@ -2083,19 +2383,19 @@
         <v>50</v>
       </c>
       <c r="I52">
-        <v>0.03721438226546</v>
+        <v>3.7214382265459998E-2</v>
       </c>
       <c r="J52">
         <v>151.6006618937655</v>
       </c>
       <c r="K52">
-        <v>78.496453</v>
+        <v>78.496453000000002</v>
       </c>
       <c r="L52">
         <v>17.47824</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>1</v>
       </c>
@@ -2106,7 +2406,7 @@
         <v>726916.255</v>
       </c>
       <c r="D53">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E53">
         <v>51</v>
@@ -2121,19 +2421,19 @@
         <v>51</v>
       </c>
       <c r="I53">
-        <v>0.03814705169783</v>
+        <v>3.8147051697830003E-2</v>
       </c>
       <c r="J53">
         <v>230.387382251665</v>
       </c>
       <c r="K53">
-        <v>78.496168</v>
+        <v>78.496167999999997</v>
       </c>
       <c r="L53">
-        <v>17.47735</v>
-      </c>
-    </row>
-    <row r="54">
+        <v>17.477350000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>1</v>
       </c>
@@ -2144,7 +2444,7 @@
         <v>726916.255</v>
       </c>
       <c r="D54">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E54">
         <v>52</v>
@@ -2159,19 +2459,19 @@
         <v>52</v>
       </c>
       <c r="I54">
-        <v>0.03853221506161</v>
+        <v>3.8532215061610003E-2</v>
       </c>
       <c r="J54">
-        <v>242.7798838963415</v>
+        <v>242.77988389634149</v>
       </c>
       <c r="K54">
-        <v>78.495786</v>
+        <v>78.495785999999995</v>
       </c>
       <c r="L54">
         <v>17.4773</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>1</v>
       </c>
@@ -2182,7 +2482,7 @@
         <v>726916.255</v>
       </c>
       <c r="D55">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E55">
         <v>53</v>
@@ -2197,19 +2497,19 @@
         <v>53</v>
       </c>
       <c r="I55">
-        <v>0.03863372536213</v>
+        <v>3.863372536213E-2</v>
       </c>
       <c r="J55">
-        <v>173.5119527120897</v>
+        <v>173.51195271208971</v>
       </c>
       <c r="K55">
-        <v>78.495717</v>
+        <v>78.495716999999999</v>
       </c>
       <c r="L55">
-        <v>17.47723</v>
-      </c>
-    </row>
-    <row r="56">
+        <v>17.477229999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>1</v>
       </c>
@@ -2220,7 +2520,7 @@
         <v>726916.255</v>
       </c>
       <c r="D56">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E56">
         <v>54</v>
@@ -2235,19 +2535,19 @@
         <v>54</v>
       </c>
       <c r="I56">
-        <v>0.03878764859547</v>
+        <v>3.8787648595470001E-2</v>
       </c>
       <c r="J56">
         <v>152.2461218825762</v>
       </c>
       <c r="K56">
-        <v>78.49584400000001</v>
+        <v>78.495844000000005</v>
       </c>
       <c r="L56">
-        <v>17.47714</v>
-      </c>
-    </row>
-    <row r="57">
+        <v>17.477139999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>1</v>
       </c>
@@ -2258,7 +2558,7 @@
         <v>726916.255</v>
       </c>
       <c r="D57">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E57">
         <v>55</v>
@@ -2273,19 +2573,19 @@
         <v>55</v>
       </c>
       <c r="I57">
-        <v>0.03905838169356</v>
+        <v>3.9058381693559997E-2</v>
       </c>
       <c r="J57">
-        <v>191.7260339986202</v>
+        <v>191.72603399862021</v>
       </c>
       <c r="K57">
-        <v>78.49584400000001</v>
+        <v>78.495844000000005</v>
       </c>
       <c r="L57">
-        <v>17.47687</v>
-      </c>
-    </row>
-    <row r="58">
+        <v>17.476870000000002</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>1</v>
       </c>
@@ -2296,7 +2596,7 @@
         <v>726916.255</v>
       </c>
       <c r="D58">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E58">
         <v>56</v>
@@ -2311,19 +2611,19 @@
         <v>56</v>
       </c>
       <c r="I58">
-        <v>0.03991420681437</v>
+        <v>3.9914206814370003E-2</v>
       </c>
       <c r="J58">
-        <v>202.9668508887289</v>
+        <v>202.96685088872891</v>
       </c>
       <c r="K58">
-        <v>78.495504</v>
+        <v>78.495503999999997</v>
       </c>
       <c r="L58">
         <v>17.47608</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>1</v>
       </c>
@@ -2334,7 +2634,7 @@
         <v>726916.255</v>
       </c>
       <c r="D59">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E59">
         <v>57</v>
@@ -2349,19 +2649,19 @@
         <v>57</v>
       </c>
       <c r="I59">
-        <v>0.04047091137693</v>
+        <v>4.0470911376929999E-2</v>
       </c>
       <c r="J59">
-        <v>193.6065353939179</v>
+        <v>193.60653539391791</v>
       </c>
       <c r="K59">
-        <v>78.49529099999999</v>
+        <v>78.495290999999995</v>
       </c>
       <c r="L59">
-        <v>17.47557</v>
-      </c>
-    </row>
-    <row r="60">
+        <v>17.475570000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>1</v>
       </c>
@@ -2372,7 +2672,7 @@
         <v>726916.255</v>
       </c>
       <c r="D60">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E60">
         <v>58</v>
@@ -2387,19 +2687,19 @@
         <v>58</v>
       </c>
       <c r="I60">
-        <v>0.04098706796388</v>
+        <v>4.0987067963879999E-2</v>
       </c>
       <c r="J60">
-        <v>173.4263925224976</v>
+        <v>173.42639252249759</v>
       </c>
       <c r="K60">
-        <v>78.495248</v>
+        <v>78.495248000000004</v>
       </c>
       <c r="L60">
-        <v>17.47506</v>
-      </c>
-    </row>
-    <row r="61">
+        <v>17.475059999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>1</v>
       </c>
@@ -2410,7 +2710,7 @@
         <v>726916.255</v>
       </c>
       <c r="D61">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E61">
         <v>59</v>
@@ -2425,19 +2725,19 @@
         <v>59</v>
       </c>
       <c r="I61">
-        <v>0.0413568839377</v>
+        <v>4.1356883937699998E-2</v>
       </c>
       <c r="J61">
-        <v>160.6927834640179</v>
+        <v>160.69278346401791</v>
       </c>
       <c r="K61">
         <v>78.495362</v>
       </c>
       <c r="L61">
-        <v>17.4747</v>
-      </c>
-    </row>
-    <row r="62">
+        <v>17.474699999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>1</v>
       </c>
@@ -2448,7 +2748,7 @@
         <v>726916.255</v>
       </c>
       <c r="D62">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E62">
         <v>60</v>
@@ -2463,19 +2763,19 @@
         <v>60</v>
       </c>
       <c r="I62">
-        <v>0.04187796429718</v>
+        <v>4.187796429718E-2</v>
       </c>
       <c r="J62">
-        <v>146.4556106737296</v>
+        <v>146.45561067372961</v>
       </c>
       <c r="K62">
-        <v>78.495546</v>
+        <v>78.495546000000004</v>
       </c>
       <c r="L62">
-        <v>17.47422</v>
-      </c>
-    </row>
-    <row r="63">
+        <v>17.474219999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>1</v>
       </c>
@@ -2486,7 +2786,7 @@
         <v>726916.255</v>
       </c>
       <c r="D63">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E63">
         <v>61</v>
@@ -2501,19 +2801,19 @@
         <v>61</v>
       </c>
       <c r="I63">
-        <v>0.04213292790597</v>
+        <v>4.2132927905970001E-2</v>
       </c>
       <c r="J63">
         <v>121.299409740085</v>
       </c>
       <c r="K63">
-        <v>78.49573100000001</v>
+        <v>78.495731000000006</v>
       </c>
       <c r="L63">
-        <v>17.47404</v>
-      </c>
-    </row>
-    <row r="64">
+        <v>17.474039999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>1</v>
       </c>
@@ -2524,7 +2824,7 @@
         <v>726916.255</v>
       </c>
       <c r="D64">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E64">
         <v>62</v>
@@ -2539,19 +2839,19 @@
         <v>62</v>
       </c>
       <c r="I64">
-        <v>0.04250805747486</v>
+        <v>4.250805747486E-2</v>
       </c>
       <c r="J64">
         <v>114.9486365453083</v>
       </c>
       <c r="K64">
-        <v>78.49608600000001</v>
+        <v>78.496086000000005</v>
       </c>
       <c r="L64">
         <v>17.47392</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>1</v>
       </c>
@@ -2562,7 +2862,7 @@
         <v>726916.255</v>
       </c>
       <c r="D65">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E65">
         <v>63</v>
@@ -2577,19 +2877,19 @@
         <v>63</v>
       </c>
       <c r="I65">
-        <v>0.04308720771147</v>
+        <v>4.3087207711470003E-2</v>
       </c>
       <c r="J65">
-        <v>163.0831514646208</v>
+        <v>163.08315146462081</v>
       </c>
       <c r="K65">
-        <v>78.496582</v>
+        <v>78.496582000000004</v>
       </c>
       <c r="L65">
         <v>17.47362</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>1</v>
       </c>
@@ -2600,7 +2900,7 @@
         <v>726916.255</v>
       </c>
       <c r="D66">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E66">
         <v>64</v>
@@ -2615,19 +2915,19 @@
         <v>64</v>
       </c>
       <c r="I66">
-        <v>0.04411968011799</v>
+        <v>4.4119680117990001E-2</v>
       </c>
       <c r="J66">
         <v>253.3686410541097</v>
       </c>
       <c r="K66">
-        <v>78.49614200000001</v>
+        <v>78.496142000000006</v>
       </c>
       <c r="L66">
         <v>17.47269</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>1</v>
       </c>
@@ -2638,7 +2938,7 @@
         <v>726916.255</v>
       </c>
       <c r="D67">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E67">
         <v>65</v>
@@ -2653,19 +2953,19 @@
         <v>65</v>
       </c>
       <c r="I67">
-        <v>0.0445858085014</v>
+        <v>4.4585808501400002E-2</v>
       </c>
       <c r="J67">
-        <v>260.7514589622954</v>
+        <v>260.75145896229537</v>
       </c>
       <c r="K67">
-        <v>78.495745</v>
+        <v>78.495744999999999</v>
       </c>
       <c r="L67">
-        <v>17.47293</v>
-      </c>
-    </row>
-    <row r="68">
+        <v>17.472930000000002</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>1</v>
       </c>
@@ -2676,7 +2976,7 @@
         <v>726916.255</v>
       </c>
       <c r="D68">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E68">
         <v>66</v>
@@ -2691,19 +2991,19 @@
         <v>66</v>
       </c>
       <c r="I68">
-        <v>0.04502750257603</v>
+        <v>4.5027502576029999E-2</v>
       </c>
       <c r="J68">
-        <v>244.993241339183</v>
+        <v>244.99324133918299</v>
       </c>
       <c r="K68">
-        <v>78.49546100000001</v>
+        <v>78.495461000000006</v>
       </c>
       <c r="L68">
         <v>17.47259</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>1</v>
       </c>
@@ -2714,7 +3014,7 @@
         <v>726916.255</v>
       </c>
       <c r="D69">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E69">
         <v>67</v>
@@ -2729,19 +3029,19 @@
         <v>67</v>
       </c>
       <c r="I69">
-        <v>0.04552421495424</v>
+        <v>4.552421495424E-2</v>
       </c>
       <c r="J69">
-        <v>269.1965020290086</v>
+        <v>269.19650202900863</v>
       </c>
       <c r="K69">
-        <v>78.494964</v>
+        <v>78.494963999999996</v>
       </c>
       <c r="L69">
         <v>17.47259</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>1</v>
       </c>
@@ -2752,7 +3052,7 @@
         <v>726916.255</v>
       </c>
       <c r="D70">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E70">
         <v>68</v>
@@ -2767,19 +3067,19 @@
         <v>68</v>
       </c>
       <c r="I70">
-        <v>0.04600692540102</v>
+        <v>4.6006925401019999E-2</v>
       </c>
       <c r="J70">
         <v>272.2974329944596</v>
       </c>
       <c r="K70">
-        <v>78.494482</v>
+        <v>78.494482000000005</v>
       </c>
       <c r="L70">
-        <v>17.47258</v>
-      </c>
-    </row>
-    <row r="71">
+        <v>17.472580000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>1</v>
       </c>
@@ -2790,7 +3090,7 @@
         <v>726916.255</v>
       </c>
       <c r="D71">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E71">
         <v>69</v>
@@ -2805,19 +3105,19 @@
         <v>69</v>
       </c>
       <c r="I71">
-        <v>0.04713467641241</v>
+        <v>4.7134676412410002E-2</v>
       </c>
       <c r="J71">
-        <v>257.3111911067112</v>
+        <v>257.31119110671119</v>
       </c>
       <c r="K71">
-        <v>78.49336099999999</v>
+        <v>78.493360999999993</v>
       </c>
       <c r="L71">
         <v>17.4727</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>1</v>
       </c>
@@ -2828,7 +3128,7 @@
         <v>726916.255</v>
       </c>
       <c r="D72">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E72">
         <v>70</v>
@@ -2843,19 +3143,19 @@
         <v>70</v>
       </c>
       <c r="I72">
-        <v>0.04788431756553</v>
+        <v>4.788431756553E-2</v>
       </c>
       <c r="J72">
-        <v>254.2102601412603</v>
+        <v>254.21026014126031</v>
       </c>
       <c r="K72">
-        <v>78.492722</v>
+        <v>78.492722000000001</v>
       </c>
       <c r="L72">
         <v>17.47231</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>1</v>
       </c>
@@ -2866,7 +3166,7 @@
         <v>726916.255</v>
       </c>
       <c r="D73">
-        <v>5197.439</v>
+        <v>5197.4390000000003</v>
       </c>
       <c r="E73">
         <v>71</v>
@@ -2881,18 +3181,19 @@
         <v>71</v>
       </c>
       <c r="I73">
-        <v>0.04789850934777</v>
+        <v>4.7898509347769999E-2</v>
       </c>
       <c r="J73">
-        <v>266.9553634181287</v>
+        <v>266.95536341812868</v>
       </c>
       <c r="K73">
-        <v>78.49270799999999</v>
+        <v>78.492707999999993</v>
       </c>
       <c r="L73">
         <v>17.47231</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>